<commit_message>
Fixed browsing experience in loaded biterdata
</commit_message>
<xml_diff>
--- a/.gitignore/rawfiles/Biterdata.xlsx
+++ b/.gitignore/rawfiles/Biterdata.xlsx
@@ -51,9 +51,6 @@
     <t>Itching, redness, and swelling at the bite site</t>
   </si>
   <si>
-    <t>Allergic reactions, including hives and anaphylaxis (in rare cases)</t>
-  </si>
-  <si>
     <t>Scratching the bites can break the skin and increase the risk of bacterial or fungal infections.</t>
   </si>
   <si>
@@ -120,9 +117,6 @@
     <t>Secondary Infections:</t>
   </si>
   <si>
-    <t>Psychological Impact:</t>
-  </si>
-  <si>
     <t>Psychological Impact</t>
   </si>
   <si>
@@ -190,6 +184,12 @@
   </si>
   <si>
     <t>Juvenile black _widow Markings</t>
+  </si>
+  <si>
+    <t>Allergic reactions</t>
+  </si>
+  <si>
+    <t>including hives and anaphylaxis (in rare cases)</t>
   </si>
 </sst>
 </file>
@@ -545,7 +545,7 @@
   <dimension ref="A1:E36"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D12" sqref="D12"/>
+      <selection sqref="A1:D26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -558,13 +558,13 @@
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="B1" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="B1" s="3" t="s">
-        <v>16</v>
-      </c>
       <c r="C1" s="4" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="D1" s="4" t="s">
         <v>0</v>
@@ -572,10 +572,10 @@
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B2" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="C2" s="1" t="s">
         <v>1</v>
@@ -586,10 +586,10 @@
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B3" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="C3" t="s">
         <v>2</v>
@@ -601,10 +601,10 @@
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B4" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="C4" t="s">
         <v>3</v>
@@ -615,10 +615,10 @@
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B5" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="C5" t="s">
         <v>4</v>
@@ -629,13 +629,13 @@
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B6" t="s">
         <v>9</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="D6" t="s">
         <v>10</v>
@@ -643,282 +643,282 @@
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B7" t="s">
         <v>9</v>
       </c>
-      <c r="C7" t="s">
-        <v>11</v>
+      <c r="C7" s="2" t="s">
+        <v>56</v>
       </c>
       <c r="D7" t="s">
-        <v>33</v>
+        <v>57</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B8" t="s">
         <v>9</v>
       </c>
       <c r="C8" t="s">
-        <v>12</v>
+        <v>32</v>
       </c>
       <c r="D8" t="s">
-        <v>34</v>
+        <v>11</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B9" t="s">
         <v>9</v>
       </c>
       <c r="C9" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="D9" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B10" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="D10" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B11" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="C11" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="D11" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B12" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="C12" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="D12" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B13" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="C13" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="D13" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B14" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="C14" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="D14" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B15" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="C15" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="D15" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B16" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="C16" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="D16" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B17" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="C17" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="D17" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B18" t="s">
         <v>9</v>
       </c>
       <c r="C18" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="D18" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B19" t="s">
         <v>9</v>
       </c>
       <c r="C19" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="D19" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B20" t="s">
         <v>9</v>
       </c>
       <c r="C20" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="D20" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B21" t="s">
         <v>9</v>
       </c>
       <c r="C21" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="D21" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B22" t="s">
         <v>9</v>
       </c>
       <c r="C22" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="D22" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B23" t="s">
         <v>9</v>
       </c>
       <c r="C23" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="D23" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B24" t="s">
         <v>9</v>
       </c>
       <c r="C24" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="D24" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B25" t="s">
         <v>9</v>
       </c>
       <c r="C25" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="D25" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B26" t="s">
         <v>9</v>
       </c>
       <c r="C26" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="D26" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
     </row>
     <row r="36" spans="2:2" ht="14.45" x14ac:dyDescent="0.35">

</xml_diff>

<commit_message>
Update plant and animal pictures
</commit_message>
<xml_diff>
--- a/.gitignore/rawfiles/Biterdata.xlsx
+++ b/.gitignore/rawfiles/Biterdata.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="720" yWindow="330" windowWidth="19425" windowHeight="12225"/>
+    <workbookView xWindow="720" yWindow="330" windowWidth="19420" windowHeight="12220"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="104" uniqueCount="58">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="253" uniqueCount="125">
   <si>
     <t>Description</t>
   </si>
@@ -190,13 +190,214 @@
   </si>
   <si>
     <t>including hives and anaphylaxis (in rare cases)</t>
+  </si>
+  <si>
+    <t>poison_hemlock</t>
+  </si>
+  <si>
+    <t>2 to 10 feet tall, with some sources stating it can reach up to 12 feet</t>
+  </si>
+  <si>
+    <t>triangular, lacy, fern-like leaf shape</t>
+  </si>
+  <si>
+    <t>grayish-brown color when mature.</t>
+  </si>
+  <si>
+    <t>body</t>
+  </si>
+  <si>
+    <t>smooth, hollow, and ridged stems with distinctive purple spots, which are covered in hairless and lacy, fern-like leaves that resemble parsley</t>
+  </si>
+  <si>
+    <t>What to do</t>
+  </si>
+  <si>
+    <t>instantly seek emergency help, get fresh air, throw out all contaiminated things, wash your skin, and wash your eyes</t>
+  </si>
+  <si>
+    <t>human_botfly</t>
+  </si>
+  <si>
+    <t>12-18mm long</t>
+  </si>
+  <si>
+    <t>Central nervous system suppression, coma, kidney failure, low blood pressure, muscle breakdown, muscle death, muscle paralysis, adnd respiratory paralysis</t>
+  </si>
+  <si>
+    <t>A chunky, bee-like aperrence</t>
+  </si>
+  <si>
+    <t>A yellow face, a metalic blue abdomen, and orange legs.</t>
+  </si>
+  <si>
+    <t>Pain and Discomfort</t>
+  </si>
+  <si>
+    <t>Inflammation and Discharge</t>
+  </si>
+  <si>
+    <t>Tissue Damage and Scarring</t>
+  </si>
+  <si>
+    <t>German shepherd</t>
+  </si>
+  <si>
+    <t>Build</t>
+  </si>
+  <si>
+    <t>Head and Face</t>
+  </si>
+  <si>
+    <t>Ears</t>
+  </si>
+  <si>
+    <t>Tail</t>
+  </si>
+  <si>
+    <t>Coat and Color</t>
+  </si>
+  <si>
+    <t>Infectious Diseases and Complications</t>
+  </si>
+  <si>
+    <t>Uncontrollable bleeding.</t>
+  </si>
+  <si>
+    <t>A deep or large wound.</t>
+  </si>
+  <si>
+    <t>Bites on the hands, face, neck, or feet.</t>
+  </si>
+  <si>
+    <t>Signs of infection like spreading redness, swelling, increasing pain, or pus.</t>
+  </si>
+  <si>
+    <t>Deep Puncture Wounds and Lacerations</t>
+  </si>
+  <si>
+    <t>Crushing Injuries and Bone Fractures</t>
+  </si>
+  <si>
+    <t>Nerve and Tendon Damage</t>
+  </si>
+  <si>
+    <t>Scarring and Disfigurement</t>
+  </si>
+  <si>
+    <t>Bacterial Infections</t>
+  </si>
+  <si>
+    <t>Cellulitis</t>
+  </si>
+  <si>
+    <t>Sepsis</t>
+  </si>
+  <si>
+    <t>Rabies</t>
+  </si>
+  <si>
+    <t>Tetanus</t>
+  </si>
+  <si>
+    <t>You should seek immediate medical care after any dog bite that breaks the skin. Prompt medical evaluation is critical to prevent severe complications, including</t>
+  </si>
+  <si>
+    <t>Psychological Effects:Post-Traumatic Stress Disorder (PTSD)</t>
+  </si>
+  <si>
+    <t>Psychological Effects:Anxiety and Fear</t>
+  </si>
+  <si>
+    <t>Psychological Effects:Depression</t>
+  </si>
+  <si>
+    <t>The developing larva creates a firm, painful, and itchy lump (known as a "warble") under the skin. A person may feel sensations of movement or sharp, stabbing pain as the larva moves or anchors itself with its spines.</t>
+  </si>
+  <si>
+    <t>A local inflammatory response with redness, swelling, and a serous, bloody, or pus-like discharge from a central breathing hole (punctum) is common.</t>
+  </si>
+  <si>
+    <t>As the larva grows, it consumes living tissue and can cause damage to the muscle. After the larva is removed and the wound heals, a significant scar may be left behind.</t>
+  </si>
+  <si>
+    <t>Males stand 24 to 26 inches tall at the shoulder and typically weigh between 65 to 90 pounds. Females are slightly smaller, standing 22 to 24 inches and weighing 50 to 70 pounds.</t>
+  </si>
+  <si>
+    <t>They have a strong, athletic build with a body that is typically longer than it is tall. The back can be straight (common in working lines) or sloped toward the hindquarters (often seen in show lines).</t>
+  </si>
+  <si>
+    <t>The head is proportionate to the body, tapering to a strong, square-cut muzzle with a black nose and powerful jaws. They have medium-sized, dark, almond-shaped eyes that convey a keen and intelligent expression.</t>
+  </si>
+  <si>
+    <t>A signature trait is their large, medium-sized ears which are broad at the base and carried erect and parallel when alert.</t>
+  </si>
+  <si>
+    <t>They possess a long, bushy tail that hangs in a slight saber-like curve when at rest.</t>
+  </si>
+  <si>
+    <t>The German Shepherd has a dense double coat to protect them in various weather. The outer coat is typically medium-length, dense, and straight or slightly wavy. Common colors include black and tan/red, black and cream, sable, and solid black.</t>
+  </si>
+  <si>
+    <t>German Shepherds have strong jaws (bite force can exceed 238 pounds per square inch) capable of inflicting deep puncture wounds and significant soft tissue damage.</t>
+  </si>
+  <si>
+    <t>The force of the bite can crush tissue and, in severe cases, break bones, especially in smaller victims like children or in sensitive areas like the hands and feet.</t>
+  </si>
+  <si>
+    <t>The deep nature of the wounds can sever or damage nerves, tendons, and muscles, potentially leading to permanent loss of function, sensation, or chronic pain in the affected area.</t>
+  </si>
+  <si>
+    <t>Severe bites often require stitches or reconstructive surgery, which can result in permanent scarring or disfigurement.</t>
+  </si>
+  <si>
+    <t>Dog mouths harbor numerous bacteria, and any bite that breaks the skin is at risk of infection.</t>
+  </si>
+  <si>
+    <t>These are the most common health concerns.</t>
+  </si>
+  <si>
+    <t>A rapidly spreading bacterial skin infection caused by bacteria likePasteurella multocida, which is common in dog saliva.</t>
+  </si>
+  <si>
+    <t>StaphandStrep Infections</t>
+  </si>
+  <si>
+    <t>Common bacterial infections that can lead to abscesses, joint swelling, and fever.</t>
+  </si>
+  <si>
+    <t>Capnocytophaga canimorsusinfection</t>
+  </si>
+  <si>
+    <t>A rare but potentially fatal infection, especially for individuals with weakened immune systems or who are asplenic (lacking a spleen). Symptoms can progress rapidly to sepsis, organ failure, andgangrene.</t>
+  </si>
+  <si>
+    <t>If an infection enters the bloodstream and spreads throughout the body, it can lead to sepsis, a life-threatening condition requiring immediate medical attention.</t>
+  </si>
+  <si>
+    <t>This is a severe, almost always fatal viral disease once symptoms appear. The risk depends on the dog's vaccination status and local rabies prevalence. If the dog is a stray or unvaccinated, post-exposure prophylaxis (PEP) is necessary.</t>
+  </si>
+  <si>
+    <t>The bacteria that cause tetanus can enter the body through a puncture wound. A tetanus shot booster may be needed if it has been more than five years since your last vaccination.</t>
+  </si>
+  <si>
+    <t>Victims may experience vivid flashbacks and intense fear.</t>
+  </si>
+  <si>
+    <t>Developing a lasting fear of dogs, which can impact daily life and social interactions.</t>
+  </si>
+  <si>
+    <t>The combination of physical injury and emotional distress can lead to depression.</t>
+  </si>
+  <si>
+    <t>If you are unsure of the dog's vaccination status or have not had a tetanus shot in the last 5-10 years.</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -207,6 +408,19 @@
     <font>
       <b/>
       <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="10"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
@@ -233,7 +447,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -241,6 +455,8 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -542,21 +758,21 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E36"/>
+  <dimension ref="A1:E65"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:D26"/>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="D56" sqref="D56"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="21.140625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="29.5703125" customWidth="1"/>
+    <col min="1" max="1" width="21.1796875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="29.54296875" customWidth="1"/>
     <col min="3" max="3" width="54" customWidth="1"/>
     <col min="4" max="4" width="90" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" ht="15" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
         <v>14</v>
       </c>
@@ -570,7 +786,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:5" ht="15" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>29</v>
       </c>
@@ -584,7 +800,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:5" ht="15" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>29</v>
       </c>
@@ -599,7 +815,7 @@
       </c>
       <c r="E3" s="1"/>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:5" ht="15" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>29</v>
       </c>
@@ -613,7 +829,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:5" ht="15" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>29</v>
       </c>
@@ -627,7 +843,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:5" ht="15" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>29</v>
       </c>
@@ -641,7 +857,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:5" ht="15" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>29</v>
       </c>
@@ -655,7 +871,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:5" ht="15" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>29</v>
       </c>
@@ -669,7 +885,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:5" ht="15" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>29</v>
       </c>
@@ -683,7 +899,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:5" ht="15" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>30</v>
       </c>
@@ -697,7 +913,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:5" ht="15" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>30</v>
       </c>
@@ -711,7 +927,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:5" ht="15" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>30</v>
       </c>
@@ -725,7 +941,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:5" ht="15" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>30</v>
       </c>
@@ -739,7 +955,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:5" ht="15" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>30</v>
       </c>
@@ -753,7 +969,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:5" ht="15" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>30</v>
       </c>
@@ -767,7 +983,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:5" ht="15" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>30</v>
       </c>
@@ -781,7 +997,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:4" ht="15" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>30</v>
       </c>
@@ -795,7 +1011,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:4" ht="15" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>30</v>
       </c>
@@ -809,7 +1025,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:4" ht="15" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>30</v>
       </c>
@@ -823,7 +1039,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:4" ht="15" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>30</v>
       </c>
@@ -837,7 +1053,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:4" ht="15" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>30</v>
       </c>
@@ -851,7 +1067,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:4" ht="15" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>30</v>
       </c>
@@ -865,7 +1081,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:4" ht="15" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>30</v>
       </c>
@@ -879,7 +1095,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:4" ht="15" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>30</v>
       </c>
@@ -893,7 +1109,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:4" ht="15" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>30</v>
       </c>
@@ -907,7 +1123,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:4" ht="15" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>30</v>
       </c>
@@ -921,8 +1137,530 @@
         <v>49</v>
       </c>
     </row>
-    <row r="36" spans="2:2" ht="14.45" x14ac:dyDescent="0.35">
-      <c r="B36" s="1"/>
+    <row r="27" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A27" s="5" t="s">
+        <v>58</v>
+      </c>
+      <c r="B27" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="C27" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="D27" s="5" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="28" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A28" s="5" t="s">
+        <v>58</v>
+      </c>
+      <c r="B28" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="C28" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="D28" s="5" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="29" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A29" s="5" t="s">
+        <v>58</v>
+      </c>
+      <c r="B29" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="C29" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="D29" s="5" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="30" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A30" s="5" t="s">
+        <v>58</v>
+      </c>
+      <c r="B30" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="C30" s="5" t="s">
+        <v>62</v>
+      </c>
+      <c r="D30" s="5" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="31" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A31" s="6" t="s">
+        <v>58</v>
+      </c>
+      <c r="B31" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="C31" s="6" t="s">
+        <v>26</v>
+      </c>
+      <c r="D31" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="32" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A32" s="5" t="s">
+        <v>58</v>
+      </c>
+      <c r="B32" s="5" t="s">
+        <v>64</v>
+      </c>
+      <c r="D32" s="5" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="33" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A33" s="5" t="s">
+        <v>66</v>
+      </c>
+      <c r="B33" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="C33" s="6" t="s">
+        <v>1</v>
+      </c>
+      <c r="D33" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="34" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A34" s="6" t="s">
+        <v>66</v>
+      </c>
+      <c r="B34" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="C34" s="6" t="s">
+        <v>2</v>
+      </c>
+      <c r="D34" s="6" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="35" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A35" s="6" t="s">
+        <v>66</v>
+      </c>
+      <c r="B35" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="C35" s="6" t="s">
+        <v>3</v>
+      </c>
+      <c r="D35" s="6" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="36" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A36" s="6" t="s">
+        <v>66</v>
+      </c>
+      <c r="B36" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="C36" t="s">
+        <v>71</v>
+      </c>
+      <c r="D36" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="37" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A37" s="6" t="s">
+        <v>66</v>
+      </c>
+      <c r="B37" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="C37" t="s">
+        <v>72</v>
+      </c>
+      <c r="D37" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="38" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A38" s="6" t="s">
+        <v>66</v>
+      </c>
+      <c r="B38" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="C38" t="s">
+        <v>73</v>
+      </c>
+      <c r="D38" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="39" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A39" s="6" t="s">
+        <v>74</v>
+      </c>
+      <c r="B39" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="C39" t="s">
+        <v>1</v>
+      </c>
+      <c r="D39" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="40" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A40" s="6" t="s">
+        <v>74</v>
+      </c>
+      <c r="B40" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="C40" t="s">
+        <v>75</v>
+      </c>
+      <c r="D40" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="41" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A41" s="6" t="s">
+        <v>74</v>
+      </c>
+      <c r="B41" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="C41" t="s">
+        <v>76</v>
+      </c>
+      <c r="D41" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="42" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A42" s="6" t="s">
+        <v>74</v>
+      </c>
+      <c r="B42" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="C42" t="s">
+        <v>77</v>
+      </c>
+      <c r="D42" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="43" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A43" s="6" t="s">
+        <v>74</v>
+      </c>
+      <c r="B43" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="C43" t="s">
+        <v>78</v>
+      </c>
+      <c r="D43" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="44" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A44" s="6" t="s">
+        <v>74</v>
+      </c>
+      <c r="B44" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="C44" t="s">
+        <v>79</v>
+      </c>
+      <c r="D44" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="45" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A45" s="6" t="s">
+        <v>74</v>
+      </c>
+      <c r="B45" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="C45" t="s">
+        <v>85</v>
+      </c>
+      <c r="D45" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="46" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A46" s="6" t="s">
+        <v>74</v>
+      </c>
+      <c r="B46" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="C46" t="s">
+        <v>86</v>
+      </c>
+      <c r="D46" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="47" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A47" s="6" t="s">
+        <v>74</v>
+      </c>
+      <c r="B47" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="C47" t="s">
+        <v>87</v>
+      </c>
+      <c r="D47" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="48" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A48" s="6" t="s">
+        <v>74</v>
+      </c>
+      <c r="B48" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="C48" t="s">
+        <v>88</v>
+      </c>
+      <c r="D48" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="49" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A49" s="6" t="s">
+        <v>74</v>
+      </c>
+      <c r="B49" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="C49" t="s">
+        <v>80</v>
+      </c>
+      <c r="D49" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="50" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A50" s="6" t="s">
+        <v>74</v>
+      </c>
+      <c r="B50" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="C50" t="s">
+        <v>89</v>
+      </c>
+      <c r="D50" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="51" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A51" s="6" t="s">
+        <v>74</v>
+      </c>
+      <c r="B51" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="C51" t="s">
+        <v>90</v>
+      </c>
+      <c r="D51" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="52" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A52" s="6" t="s">
+        <v>74</v>
+      </c>
+      <c r="B52" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="C52" t="s">
+        <v>114</v>
+      </c>
+      <c r="D52" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="53" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A53" s="6" t="s">
+        <v>74</v>
+      </c>
+      <c r="B53" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="C53" t="s">
+        <v>116</v>
+      </c>
+      <c r="D53" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="54" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A54" s="6" t="s">
+        <v>74</v>
+      </c>
+      <c r="B54" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="C54" t="s">
+        <v>91</v>
+      </c>
+      <c r="D54" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="55" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A55" s="6" t="s">
+        <v>74</v>
+      </c>
+      <c r="B55" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="C55" t="s">
+        <v>92</v>
+      </c>
+      <c r="D55" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="56" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A56" s="6" t="s">
+        <v>74</v>
+      </c>
+      <c r="B56" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="C56" t="s">
+        <v>93</v>
+      </c>
+      <c r="D56" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="57" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A57" s="6" t="s">
+        <v>74</v>
+      </c>
+      <c r="B57" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="C57" t="s">
+        <v>95</v>
+      </c>
+      <c r="D57" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="58" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A58" s="6" t="s">
+        <v>74</v>
+      </c>
+      <c r="B58" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="C58" t="s">
+        <v>96</v>
+      </c>
+      <c r="D58" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="59" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A59" s="6" t="s">
+        <v>74</v>
+      </c>
+      <c r="B59" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="C59" t="s">
+        <v>97</v>
+      </c>
+      <c r="D59" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="60" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A60" s="6" t="s">
+        <v>74</v>
+      </c>
+      <c r="B60" t="s">
+        <v>64</v>
+      </c>
+      <c r="D60" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="61" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A61" s="6" t="s">
+        <v>74</v>
+      </c>
+      <c r="B61" t="s">
+        <v>64</v>
+      </c>
+      <c r="D61" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="62" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A62" s="6" t="s">
+        <v>74</v>
+      </c>
+      <c r="B62" t="s">
+        <v>64</v>
+      </c>
+      <c r="D62" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="63" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A63" s="6" t="s">
+        <v>74</v>
+      </c>
+      <c r="B63" t="s">
+        <v>64</v>
+      </c>
+      <c r="D63" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="64" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A64" s="6" t="s">
+        <v>74</v>
+      </c>
+      <c r="B64" t="s">
+        <v>64</v>
+      </c>
+      <c r="D64" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="65" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A65" s="6" t="s">
+        <v>74</v>
+      </c>
+      <c r="B65" t="s">
+        <v>64</v>
+      </c>
+      <c r="D65" t="s">
+        <v>124</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -936,7 +1674,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -948,7 +1686,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Add search function, trial 1
</commit_message>
<xml_diff>
--- a/.gitignore/rawfiles/Biterdata.xlsx
+++ b/.gitignore/rawfiles/Biterdata.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="720" yWindow="330" windowWidth="19420" windowHeight="12220"/>
+    <workbookView xWindow="720" yWindow="330" windowWidth="19425" windowHeight="12225"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="253" uniqueCount="125">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="293" uniqueCount="135">
   <si>
     <t>Description</t>
   </si>
@@ -240,9 +240,6 @@
     <t>Tissue Damage and Scarring</t>
   </si>
   <si>
-    <t>German shepherd</t>
-  </si>
-  <si>
     <t>Build</t>
   </si>
   <si>
@@ -391,6 +388,39 @@
   </si>
   <si>
     <t>If you are unsure of the dog's vaccination status or have not had a tetanus shot in the last 5-10 years.</t>
+  </si>
+  <si>
+    <t>Class</t>
+  </si>
+  <si>
+    <t>Plants</t>
+  </si>
+  <si>
+    <t>Bugs</t>
+  </si>
+  <si>
+    <t>Animals</t>
+  </si>
+  <si>
+    <t>tiny,reddish,brown,bed,itch</t>
+  </si>
+  <si>
+    <t>black,dark brown,spider,hourglass,red mark,venemous,swell,numbness,muscle ache</t>
+  </si>
+  <si>
+    <t>triangular, lacy, fern like,grayish-brown,smooth,hollow stem,purple spot,coma,low blood pressure</t>
+  </si>
+  <si>
+    <t>chunky,bee-like,yellow,blue abdomen,pain,ichy,swell,larva</t>
+  </si>
+  <si>
+    <t>dog,black,big dog,black back,big ear,large ear,rabies,tentanus</t>
+  </si>
+  <si>
+    <t>OtherKeywords</t>
+  </si>
+  <si>
+    <t>German_shepherd</t>
   </si>
 </sst>
 </file>
@@ -758,21 +788,21 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E65"/>
+  <dimension ref="A1:E75"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="D56" sqref="D56"/>
+    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="D3" sqref="D3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="21.1796875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="29.54296875" customWidth="1"/>
+    <col min="1" max="1" width="21.140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="29.5703125" customWidth="1"/>
     <col min="3" max="3" width="54" customWidth="1"/>
     <col min="4" max="4" width="90" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" ht="15" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
         <v>14</v>
       </c>
@@ -786,50 +816,49 @@
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:5" ht="15" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>29</v>
       </c>
-      <c r="B2" t="s">
-        <v>16</v>
-      </c>
-      <c r="C2" s="1" t="s">
-        <v>1</v>
+      <c r="B2" s="3" t="s">
+        <v>124</v>
+      </c>
+      <c r="C2" s="3" t="s">
+        <v>124</v>
       </c>
       <c r="D2" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5" ht="15" x14ac:dyDescent="0.25">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>29</v>
       </c>
-      <c r="B3" t="s">
-        <v>16</v>
-      </c>
-      <c r="C3" t="s">
-        <v>2</v>
-      </c>
-      <c r="D3" t="s">
-        <v>5</v>
-      </c>
-      <c r="E3" s="1"/>
-    </row>
-    <row r="4" spans="1:5" ht="15" x14ac:dyDescent="0.25">
+      <c r="B3" s="3" t="s">
+        <v>133</v>
+      </c>
+      <c r="C3" s="3" t="s">
+        <v>133</v>
+      </c>
+      <c r="D3" s="4" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>29</v>
       </c>
       <c r="B4" t="s">
         <v>16</v>
       </c>
-      <c r="C4" t="s">
-        <v>3</v>
+      <c r="C4" s="1" t="s">
+        <v>1</v>
       </c>
       <c r="D4" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5" ht="15" x14ac:dyDescent="0.25">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>29</v>
       </c>
@@ -837,139 +866,140 @@
         <v>16</v>
       </c>
       <c r="C5" t="s">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="D5" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="6" spans="1:5" ht="15" x14ac:dyDescent="0.25">
+        <v>5</v>
+      </c>
+      <c r="E5" s="1"/>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>29</v>
       </c>
       <c r="B6" t="s">
-        <v>9</v>
-      </c>
-      <c r="C6" s="2" t="s">
-        <v>31</v>
+        <v>16</v>
+      </c>
+      <c r="C6" t="s">
+        <v>3</v>
       </c>
       <c r="D6" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="7" spans="1:5" ht="15" x14ac:dyDescent="0.25">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>29</v>
       </c>
       <c r="B7" t="s">
-        <v>9</v>
-      </c>
-      <c r="C7" s="2" t="s">
-        <v>56</v>
+        <v>16</v>
+      </c>
+      <c r="C7" t="s">
+        <v>4</v>
       </c>
       <c r="D7" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="8" spans="1:5" ht="15" x14ac:dyDescent="0.25">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>29</v>
       </c>
       <c r="B8" t="s">
         <v>9</v>
       </c>
-      <c r="C8" t="s">
-        <v>32</v>
+      <c r="C8" s="2" t="s">
+        <v>31</v>
       </c>
       <c r="D8" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="9" spans="1:5" ht="15" x14ac:dyDescent="0.25">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>29</v>
       </c>
       <c r="B9" t="s">
         <v>9</v>
       </c>
-      <c r="C9" t="s">
+      <c r="C9" s="2" t="s">
+        <v>56</v>
+      </c>
+      <c r="D9" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>29</v>
+      </c>
+      <c r="B10" t="s">
+        <v>9</v>
+      </c>
+      <c r="C10" t="s">
+        <v>32</v>
+      </c>
+      <c r="D10" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>29</v>
+      </c>
+      <c r="B11" t="s">
+        <v>9</v>
+      </c>
+      <c r="C11" t="s">
         <v>33</v>
       </c>
-      <c r="D9" t="s">
+      <c r="D11" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="10" spans="1:5" ht="15" x14ac:dyDescent="0.25">
-      <c r="A10" t="s">
-        <v>30</v>
-      </c>
-      <c r="B10" t="s">
-        <v>16</v>
-      </c>
-      <c r="C10" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="D10" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="11" spans="1:5" ht="15" x14ac:dyDescent="0.25">
-      <c r="A11" t="s">
-        <v>30</v>
-      </c>
-      <c r="B11" t="s">
-        <v>16</v>
-      </c>
-      <c r="C11" t="s">
-        <v>51</v>
-      </c>
-      <c r="D11" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="12" spans="1:5" ht="15" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>30</v>
       </c>
       <c r="B12" t="s">
-        <v>16</v>
+        <v>124</v>
       </c>
       <c r="C12" t="s">
-        <v>52</v>
+        <v>124</v>
       </c>
       <c r="D12" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="13" spans="1:5" ht="15" x14ac:dyDescent="0.25">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>30</v>
       </c>
-      <c r="B13" t="s">
-        <v>16</v>
-      </c>
-      <c r="C13" t="s">
-        <v>38</v>
-      </c>
-      <c r="D13" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="14" spans="1:5" ht="15" x14ac:dyDescent="0.25">
+      <c r="B13" s="3" t="s">
+        <v>133</v>
+      </c>
+      <c r="C13" s="3" t="s">
+        <v>133</v>
+      </c>
+      <c r="D13" s="4" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>30</v>
       </c>
       <c r="B14" t="s">
         <v>16</v>
       </c>
-      <c r="C14" t="s">
-        <v>53</v>
+      <c r="C14" s="1" t="s">
+        <v>34</v>
       </c>
       <c r="D14" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="15" spans="1:5" ht="15" x14ac:dyDescent="0.25">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>30</v>
       </c>
@@ -977,13 +1007,13 @@
         <v>16</v>
       </c>
       <c r="C15" t="s">
-        <v>54</v>
+        <v>51</v>
       </c>
       <c r="D15" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="16" spans="1:5" ht="15" x14ac:dyDescent="0.25">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>30</v>
       </c>
@@ -991,13 +1021,13 @@
         <v>16</v>
       </c>
       <c r="C16" t="s">
-        <v>41</v>
+        <v>52</v>
       </c>
       <c r="D16" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="17" spans="1:4" ht="15" x14ac:dyDescent="0.25">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>30</v>
       </c>
@@ -1005,69 +1035,69 @@
         <v>16</v>
       </c>
       <c r="C17" t="s">
-        <v>55</v>
+        <v>38</v>
       </c>
       <c r="D17" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="18" spans="1:4" ht="15" x14ac:dyDescent="0.25">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>30</v>
       </c>
       <c r="B18" t="s">
-        <v>9</v>
+        <v>16</v>
       </c>
       <c r="C18" t="s">
-        <v>17</v>
+        <v>53</v>
       </c>
       <c r="D18" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="19" spans="1:4" ht="15" x14ac:dyDescent="0.25">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>30</v>
       </c>
       <c r="B19" t="s">
-        <v>9</v>
+        <v>16</v>
       </c>
       <c r="C19" t="s">
-        <v>18</v>
+        <v>54</v>
       </c>
       <c r="D19" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="20" spans="1:4" ht="15" x14ac:dyDescent="0.25">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>30</v>
       </c>
       <c r="B20" t="s">
-        <v>9</v>
+        <v>16</v>
       </c>
       <c r="C20" t="s">
-        <v>19</v>
+        <v>41</v>
       </c>
       <c r="D20" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="21" spans="1:4" ht="15" x14ac:dyDescent="0.25">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>30</v>
       </c>
       <c r="B21" t="s">
-        <v>9</v>
+        <v>16</v>
       </c>
       <c r="C21" t="s">
-        <v>20</v>
+        <v>55</v>
       </c>
       <c r="D21" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="22" spans="1:4" ht="15" x14ac:dyDescent="0.25">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>30</v>
       </c>
@@ -1075,13 +1105,13 @@
         <v>9</v>
       </c>
       <c r="C22" t="s">
-        <v>24</v>
+        <v>17</v>
       </c>
       <c r="D22" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="23" spans="1:4" ht="15" x14ac:dyDescent="0.25">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>30</v>
       </c>
@@ -1089,13 +1119,13 @@
         <v>9</v>
       </c>
       <c r="C23" t="s">
-        <v>25</v>
+        <v>18</v>
       </c>
       <c r="D23" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="24" spans="1:4" ht="15" x14ac:dyDescent="0.25">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>30</v>
       </c>
@@ -1103,13 +1133,13 @@
         <v>9</v>
       </c>
       <c r="C24" t="s">
-        <v>26</v>
+        <v>19</v>
       </c>
       <c r="D24" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="25" spans="1:4" ht="15" x14ac:dyDescent="0.25">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>30</v>
       </c>
@@ -1117,13 +1147,13 @@
         <v>9</v>
       </c>
       <c r="C25" t="s">
-        <v>27</v>
+        <v>20</v>
       </c>
       <c r="D25" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="26" spans="1:4" ht="15" x14ac:dyDescent="0.25">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>30</v>
       </c>
@@ -1131,535 +1161,675 @@
         <v>9</v>
       </c>
       <c r="C26" t="s">
+        <v>24</v>
+      </c>
+      <c r="D26" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A27" t="s">
+        <v>30</v>
+      </c>
+      <c r="B27" t="s">
+        <v>9</v>
+      </c>
+      <c r="C27" t="s">
+        <v>25</v>
+      </c>
+      <c r="D27" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A28" t="s">
+        <v>30</v>
+      </c>
+      <c r="B28" t="s">
+        <v>9</v>
+      </c>
+      <c r="C28" t="s">
+        <v>26</v>
+      </c>
+      <c r="D28" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A29" t="s">
+        <v>30</v>
+      </c>
+      <c r="B29" t="s">
+        <v>9</v>
+      </c>
+      <c r="C29" t="s">
+        <v>27</v>
+      </c>
+      <c r="D29" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="30" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A30" t="s">
+        <v>30</v>
+      </c>
+      <c r="B30" t="s">
+        <v>9</v>
+      </c>
+      <c r="C30" t="s">
         <v>28</v>
       </c>
-      <c r="D26" t="s">
+      <c r="D30" t="s">
         <v>49</v>
       </c>
     </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A27" s="5" t="s">
+    <row r="31" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A31" s="5" t="s">
         <v>58</v>
       </c>
-      <c r="B27" s="5" t="s">
-        <v>16</v>
-      </c>
-      <c r="C27" s="5" t="s">
-        <v>1</v>
-      </c>
-      <c r="D27" s="5" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A28" s="5" t="s">
-        <v>58</v>
-      </c>
-      <c r="B28" s="5" t="s">
-        <v>16</v>
-      </c>
-      <c r="C28" s="5" t="s">
-        <v>2</v>
-      </c>
-      <c r="D28" s="5" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A29" s="5" t="s">
-        <v>58</v>
-      </c>
-      <c r="B29" s="5" t="s">
-        <v>16</v>
-      </c>
-      <c r="C29" s="5" t="s">
-        <v>3</v>
-      </c>
-      <c r="D29" s="5" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="30" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A30" s="5" t="s">
-        <v>58</v>
-      </c>
-      <c r="B30" s="5" t="s">
-        <v>16</v>
-      </c>
-      <c r="C30" s="5" t="s">
-        <v>62</v>
-      </c>
-      <c r="D30" s="5" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="31" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A31" s="6" t="s">
-        <v>58</v>
-      </c>
-      <c r="B31" s="5" t="s">
-        <v>9</v>
-      </c>
-      <c r="C31" s="6" t="s">
-        <v>26</v>
+      <c r="B31" t="s">
+        <v>124</v>
+      </c>
+      <c r="C31" t="s">
+        <v>124</v>
       </c>
       <c r="D31" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="32" spans="1:4" x14ac:dyDescent="0.35">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="32" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A32" s="5" t="s">
         <v>58</v>
       </c>
       <c r="B32" s="5" t="s">
+        <v>133</v>
+      </c>
+      <c r="C32" t="s">
+        <v>133</v>
+      </c>
+      <c r="D32" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="33" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A33" s="5" t="s">
+        <v>58</v>
+      </c>
+      <c r="B33" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="C33" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="D33" s="5" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="34" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A34" s="5" t="s">
+        <v>58</v>
+      </c>
+      <c r="B34" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="C34" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="D34" s="5" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="35" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A35" s="5" t="s">
+        <v>58</v>
+      </c>
+      <c r="B35" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="C35" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="D35" s="5" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="36" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A36" s="5" t="s">
+        <v>58</v>
+      </c>
+      <c r="B36" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="C36" s="5" t="s">
+        <v>62</v>
+      </c>
+      <c r="D36" s="5" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="37" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A37" s="6" t="s">
+        <v>58</v>
+      </c>
+      <c r="B37" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="C37" s="6" t="s">
+        <v>26</v>
+      </c>
+      <c r="D37" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="38" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A38" s="5" t="s">
+        <v>58</v>
+      </c>
+      <c r="B38" s="5" t="s">
         <v>64</v>
       </c>
-      <c r="D32" s="5" t="s">
+      <c r="D38" s="5" t="s">
         <v>65</v>
       </c>
     </row>
-    <row r="33" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A33" s="5" t="s">
+    <row r="39" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A39" s="5" t="s">
         <v>66</v>
       </c>
-      <c r="B33" s="5" t="s">
-        <v>16</v>
-      </c>
-      <c r="C33" s="6" t="s">
+      <c r="B39" s="5" t="s">
+        <v>124</v>
+      </c>
+      <c r="C39" s="6" t="s">
+        <v>124</v>
+      </c>
+      <c r="D39" s="5" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="40" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A40" s="5" t="s">
+        <v>66</v>
+      </c>
+      <c r="B40" s="5" t="s">
+        <v>133</v>
+      </c>
+      <c r="C40" s="6" t="s">
+        <v>133</v>
+      </c>
+      <c r="D40" s="5" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="41" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A41" s="5" t="s">
+        <v>66</v>
+      </c>
+      <c r="B41" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="C41" s="6" t="s">
         <v>1</v>
       </c>
-      <c r="D33" t="s">
+      <c r="D41" t="s">
         <v>67</v>
       </c>
     </row>
-    <row r="34" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A34" s="6" t="s">
+    <row r="42" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A42" s="6" t="s">
         <v>66</v>
       </c>
-      <c r="B34" s="6" t="s">
-        <v>16</v>
-      </c>
-      <c r="C34" s="6" t="s">
+      <c r="B42" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="C42" s="6" t="s">
         <v>2</v>
       </c>
-      <c r="D34" s="6" t="s">
+      <c r="D42" s="6" t="s">
         <v>69</v>
       </c>
     </row>
-    <row r="35" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A35" s="6" t="s">
+    <row r="43" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A43" s="6" t="s">
         <v>66</v>
       </c>
-      <c r="B35" s="6" t="s">
-        <v>16</v>
-      </c>
-      <c r="C35" s="6" t="s">
+      <c r="B43" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="C43" s="6" t="s">
         <v>3</v>
       </c>
-      <c r="D35" s="6" t="s">
+      <c r="D43" s="6" t="s">
         <v>70</v>
       </c>
     </row>
-    <row r="36" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A36" s="6" t="s">
+    <row r="44" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A44" s="6" t="s">
         <v>66</v>
       </c>
-      <c r="B36" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="C36" t="s">
+      <c r="B44" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="C44" t="s">
         <v>71</v>
       </c>
-      <c r="D36" t="s">
+      <c r="D44" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="45" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A45" s="6" t="s">
+        <v>66</v>
+      </c>
+      <c r="B45" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="C45" t="s">
+        <v>72</v>
+      </c>
+      <c r="D45" t="s">
         <v>98</v>
       </c>
     </row>
-    <row r="37" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A37" s="6" t="s">
+    <row r="46" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A46" s="6" t="s">
         <v>66</v>
       </c>
-      <c r="B37" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="C37" t="s">
-        <v>72</v>
-      </c>
-      <c r="D37" t="s">
+      <c r="B46" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="C46" t="s">
+        <v>73</v>
+      </c>
+      <c r="D46" t="s">
         <v>99</v>
       </c>
     </row>
-    <row r="38" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A38" s="6" t="s">
-        <v>66</v>
-      </c>
-      <c r="B38" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="C38" t="s">
-        <v>73</v>
-      </c>
-      <c r="D38" t="s">
+    <row r="47" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A47" s="6" t="s">
+        <v>134</v>
+      </c>
+      <c r="B47" s="1" t="s">
+        <v>124</v>
+      </c>
+      <c r="C47" t="s">
+        <v>124</v>
+      </c>
+      <c r="D47" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="48" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A48" s="6" t="s">
+        <v>134</v>
+      </c>
+      <c r="B48" s="1" t="s">
+        <v>133</v>
+      </c>
+      <c r="C48" t="s">
+        <v>133</v>
+      </c>
+      <c r="D48" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="49" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A49" s="6" t="s">
+        <v>134</v>
+      </c>
+      <c r="B49" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="C49" t="s">
+        <v>1</v>
+      </c>
+      <c r="D49" t="s">
         <v>100</v>
       </c>
     </row>
-    <row r="39" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A39" s="6" t="s">
+    <row r="50" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A50" s="6" t="s">
+        <v>134</v>
+      </c>
+      <c r="B50" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="C50" t="s">
         <v>74</v>
       </c>
-      <c r="B39" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="C39" t="s">
-        <v>1</v>
-      </c>
-      <c r="D39" t="s">
+      <c r="D50" t="s">
         <v>101</v>
       </c>
     </row>
-    <row r="40" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A40" s="6" t="s">
-        <v>74</v>
-      </c>
-      <c r="B40" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="C40" t="s">
+    <row r="51" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A51" s="6" t="s">
+        <v>134</v>
+      </c>
+      <c r="B51" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="C51" t="s">
         <v>75</v>
       </c>
-      <c r="D40" t="s">
+      <c r="D51" t="s">
         <v>102</v>
       </c>
     </row>
-    <row r="41" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A41" s="6" t="s">
-        <v>74</v>
-      </c>
-      <c r="B41" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="C41" t="s">
+    <row r="52" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A52" s="6" t="s">
+        <v>134</v>
+      </c>
+      <c r="B52" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="C52" t="s">
         <v>76</v>
       </c>
-      <c r="D41" t="s">
+      <c r="D52" t="s">
         <v>103</v>
       </c>
     </row>
-    <row r="42" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A42" s="6" t="s">
-        <v>74</v>
-      </c>
-      <c r="B42" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="C42" t="s">
+    <row r="53" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A53" s="6" t="s">
+        <v>134</v>
+      </c>
+      <c r="B53" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="C53" t="s">
         <v>77</v>
       </c>
-      <c r="D42" t="s">
+      <c r="D53" t="s">
         <v>104</v>
       </c>
     </row>
-    <row r="43" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A43" s="6" t="s">
-        <v>74</v>
-      </c>
-      <c r="B43" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="C43" t="s">
+    <row r="54" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A54" s="6" t="s">
+        <v>134</v>
+      </c>
+      <c r="B54" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="C54" t="s">
         <v>78</v>
       </c>
-      <c r="D43" t="s">
+      <c r="D54" t="s">
         <v>105</v>
       </c>
     </row>
-    <row r="44" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A44" s="6" t="s">
-        <v>74</v>
-      </c>
-      <c r="B44" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="C44" t="s">
+    <row r="55" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A55" s="6" t="s">
+        <v>134</v>
+      </c>
+      <c r="B55" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="C55" t="s">
+        <v>84</v>
+      </c>
+      <c r="D55" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="56" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A56" s="6" t="s">
+        <v>134</v>
+      </c>
+      <c r="B56" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="C56" t="s">
+        <v>85</v>
+      </c>
+      <c r="D56" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="57" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A57" s="6" t="s">
+        <v>134</v>
+      </c>
+      <c r="B57" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="C57" t="s">
+        <v>86</v>
+      </c>
+      <c r="D57" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="58" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A58" s="6" t="s">
+        <v>134</v>
+      </c>
+      <c r="B58" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="C58" t="s">
+        <v>87</v>
+      </c>
+      <c r="D58" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="59" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A59" s="6" t="s">
+        <v>134</v>
+      </c>
+      <c r="B59" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="C59" t="s">
         <v>79</v>
       </c>
-      <c r="D44" t="s">
-        <v>106</v>
-      </c>
-    </row>
-    <row r="45" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A45" s="6" t="s">
-        <v>74</v>
-      </c>
-      <c r="B45" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="C45" t="s">
-        <v>85</v>
-      </c>
-      <c r="D45" t="s">
-        <v>107</v>
-      </c>
-    </row>
-    <row r="46" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A46" s="6" t="s">
-        <v>74</v>
-      </c>
-      <c r="B46" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="C46" t="s">
-        <v>86</v>
-      </c>
-      <c r="D46" t="s">
-        <v>108</v>
-      </c>
-    </row>
-    <row r="47" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A47" s="6" t="s">
-        <v>74</v>
-      </c>
-      <c r="B47" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="C47" t="s">
-        <v>87</v>
-      </c>
-      <c r="D47" t="s">
-        <v>109</v>
-      </c>
-    </row>
-    <row r="48" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A48" s="6" t="s">
-        <v>74</v>
-      </c>
-      <c r="B48" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="C48" t="s">
+      <c r="D59" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="60" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A60" s="6" t="s">
+        <v>134</v>
+      </c>
+      <c r="B60" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="C60" t="s">
         <v>88</v>
       </c>
-      <c r="D48" t="s">
-        <v>110</v>
-      </c>
-    </row>
-    <row r="49" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A49" s="6" t="s">
-        <v>74</v>
-      </c>
-      <c r="B49" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="C49" t="s">
+      <c r="D60" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="61" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A61" s="6" t="s">
+        <v>134</v>
+      </c>
+      <c r="B61" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="C61" t="s">
+        <v>89</v>
+      </c>
+      <c r="D61" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="62" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A62" s="6" t="s">
+        <v>134</v>
+      </c>
+      <c r="B62" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="C62" t="s">
+        <v>113</v>
+      </c>
+      <c r="D62" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="63" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A63" s="6" t="s">
+        <v>134</v>
+      </c>
+      <c r="B63" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="C63" t="s">
+        <v>115</v>
+      </c>
+      <c r="D63" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="64" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A64" s="6" t="s">
+        <v>134</v>
+      </c>
+      <c r="B64" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="C64" t="s">
+        <v>90</v>
+      </c>
+      <c r="D64" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="65" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A65" s="6" t="s">
+        <v>134</v>
+      </c>
+      <c r="B65" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="C65" t="s">
+        <v>91</v>
+      </c>
+      <c r="D65" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="66" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A66" s="6" t="s">
+        <v>134</v>
+      </c>
+      <c r="B66" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="C66" t="s">
+        <v>92</v>
+      </c>
+      <c r="D66" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="67" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A67" s="6" t="s">
+        <v>134</v>
+      </c>
+      <c r="B67" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="C67" t="s">
+        <v>94</v>
+      </c>
+      <c r="D67" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="68" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A68" s="6" t="s">
+        <v>134</v>
+      </c>
+      <c r="B68" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="C68" t="s">
+        <v>95</v>
+      </c>
+      <c r="D68" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="69" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A69" s="6" t="s">
+        <v>134</v>
+      </c>
+      <c r="B69" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="C69" t="s">
+        <v>96</v>
+      </c>
+      <c r="D69" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="70" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A70" s="6" t="s">
+        <v>134</v>
+      </c>
+      <c r="B70" t="s">
+        <v>64</v>
+      </c>
+      <c r="D70" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="71" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A71" s="6" t="s">
+        <v>134</v>
+      </c>
+      <c r="B71" t="s">
+        <v>64</v>
+      </c>
+      <c r="D71" t="s">
         <v>80</v>
       </c>
-      <c r="D49" t="s">
-        <v>111</v>
-      </c>
-    </row>
-    <row r="50" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A50" s="6" t="s">
-        <v>74</v>
-      </c>
-      <c r="B50" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="C50" t="s">
-        <v>89</v>
-      </c>
-      <c r="D50" t="s">
-        <v>112</v>
-      </c>
-    </row>
-    <row r="51" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A51" s="6" t="s">
-        <v>74</v>
-      </c>
-      <c r="B51" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="C51" t="s">
-        <v>90</v>
-      </c>
-      <c r="D51" t="s">
-        <v>113</v>
-      </c>
-    </row>
-    <row r="52" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A52" s="6" t="s">
-        <v>74</v>
-      </c>
-      <c r="B52" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="C52" t="s">
-        <v>114</v>
-      </c>
-      <c r="D52" t="s">
-        <v>115</v>
-      </c>
-    </row>
-    <row r="53" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A53" s="6" t="s">
-        <v>74</v>
-      </c>
-      <c r="B53" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="C53" t="s">
-        <v>116</v>
-      </c>
-      <c r="D53" t="s">
-        <v>117</v>
-      </c>
-    </row>
-    <row r="54" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A54" s="6" t="s">
-        <v>74</v>
-      </c>
-      <c r="B54" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="C54" t="s">
-        <v>91</v>
-      </c>
-      <c r="D54" t="s">
-        <v>118</v>
-      </c>
-    </row>
-    <row r="55" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A55" s="6" t="s">
-        <v>74</v>
-      </c>
-      <c r="B55" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="C55" t="s">
-        <v>92</v>
-      </c>
-      <c r="D55" t="s">
-        <v>119</v>
-      </c>
-    </row>
-    <row r="56" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A56" s="6" t="s">
-        <v>74</v>
-      </c>
-      <c r="B56" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="C56" t="s">
-        <v>93</v>
-      </c>
-      <c r="D56" t="s">
-        <v>120</v>
-      </c>
-    </row>
-    <row r="57" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A57" s="6" t="s">
-        <v>74</v>
-      </c>
-      <c r="B57" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="C57" t="s">
-        <v>95</v>
-      </c>
-      <c r="D57" t="s">
-        <v>121</v>
-      </c>
-    </row>
-    <row r="58" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A58" s="6" t="s">
-        <v>74</v>
-      </c>
-      <c r="B58" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="C58" t="s">
-        <v>96</v>
-      </c>
-      <c r="D58" t="s">
-        <v>122</v>
-      </c>
-    </row>
-    <row r="59" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A59" s="6" t="s">
-        <v>74</v>
-      </c>
-      <c r="B59" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="C59" t="s">
-        <v>97</v>
-      </c>
-      <c r="D59" t="s">
+    </row>
+    <row r="72" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A72" s="6" t="s">
+        <v>134</v>
+      </c>
+      <c r="B72" t="s">
+        <v>64</v>
+      </c>
+      <c r="D72" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="73" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A73" s="6" t="s">
+        <v>134</v>
+      </c>
+      <c r="B73" t="s">
+        <v>64</v>
+      </c>
+      <c r="D73" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="74" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A74" s="6" t="s">
+        <v>134</v>
+      </c>
+      <c r="B74" t="s">
+        <v>64</v>
+      </c>
+      <c r="D74" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="75" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A75" s="6" t="s">
+        <v>134</v>
+      </c>
+      <c r="B75" t="s">
+        <v>64</v>
+      </c>
+      <c r="D75" t="s">
         <v>123</v>
-      </c>
-    </row>
-    <row r="60" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A60" s="6" t="s">
-        <v>74</v>
-      </c>
-      <c r="B60" t="s">
-        <v>64</v>
-      </c>
-      <c r="D60" t="s">
-        <v>94</v>
-      </c>
-    </row>
-    <row r="61" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A61" s="6" t="s">
-        <v>74</v>
-      </c>
-      <c r="B61" t="s">
-        <v>64</v>
-      </c>
-      <c r="D61" t="s">
-        <v>81</v>
-      </c>
-    </row>
-    <row r="62" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A62" s="6" t="s">
-        <v>74</v>
-      </c>
-      <c r="B62" t="s">
-        <v>64</v>
-      </c>
-      <c r="D62" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="63" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A63" s="6" t="s">
-        <v>74</v>
-      </c>
-      <c r="B63" t="s">
-        <v>64</v>
-      </c>
-      <c r="D63" t="s">
-        <v>83</v>
-      </c>
-    </row>
-    <row r="64" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A64" s="6" t="s">
-        <v>74</v>
-      </c>
-      <c r="B64" t="s">
-        <v>64</v>
-      </c>
-      <c r="D64" t="s">
-        <v>84</v>
-      </c>
-    </row>
-    <row r="65" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A65" s="6" t="s">
-        <v>74</v>
-      </c>
-      <c r="B65" t="s">
-        <v>64</v>
-      </c>
-      <c r="D65" t="s">
-        <v>124</v>
       </c>
     </row>
   </sheetData>
@@ -1674,7 +1844,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -1686,7 +1856,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Add search function, trial 2
</commit_message>
<xml_diff>
--- a/.gitignore/rawfiles/Biterdata.xlsx
+++ b/.gitignore/rawfiles/Biterdata.xlsx
@@ -420,7 +420,7 @@
     <t>OtherKeywords</t>
   </si>
   <si>
-    <t>German_shepherd</t>
+    <t>German_Shepherd</t>
   </si>
 </sst>
 </file>
@@ -790,8 +790,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E75"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="D3" sqref="D3"/>
+    <sheetView tabSelected="1" topLeftCell="A46" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="A75" sqref="A75"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>